<commit_message>
Agregado recientemente usuario y clave de VisualCont!
</commit_message>
<xml_diff>
--- a/Claves personales.xlsx
+++ b/Claves personales.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
   <si>
     <t>ENTIDAD</t>
   </si>
@@ -197,6 +197,12 @@
   </si>
   <si>
     <t>Canva</t>
+  </si>
+  <si>
+    <t>visualcont</t>
+  </si>
+  <si>
+    <t>usuarioroot</t>
   </si>
 </sst>
 </file>
@@ -619,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:E38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,9 +1070,15 @@
       <c r="B36" s="8">
         <v>31</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
+      <c r="C36" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" s="1">
+        <v>123</v>
+      </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="1">

</xml_diff>